<commit_message>
Ok went ahead and applied that bug fix to the week generation. Also while I was around and thinking about, applied whatever changes were necessary to get offblock rules working on regular activities. Note: this will work regardless of whether or not that activity has a specialist (we figure that theres probably a usecase for 'the playground is occupied' or 'this activity is off limits at this time'). Also found a little not error but just input flaw with the week example so fixed that on the example file
</commit_message>
<xml_diff>
--- a/CampScheduler/CampScheduler/CampSchedulerInputExamples.xlsx
+++ b/CampScheduler/CampScheduler/CampSchedulerInputExamples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dryan\OneDrive\Documents\GitHub\CampScheduler\CampScheduler\CampScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D25CB1-0F55-4354-ADCB-1D39F96766BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12193CC4-5B14-4972-8D4B-BDB2D637D012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{0861955A-A212-4BF4-8127-4D8CB03931E6}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="1" activeTab="4" xr2:uid="{0861955A-A212-4BF4-8127-4D8CB03931E6}"/>
   </bookViews>
   <sheets>
     <sheet name="DayInputEmpty" sheetId="2" r:id="rId1"/>
@@ -1787,7 +1787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482F8C11-A64A-4254-A7A9-8102F6EDAC68}">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="41" workbookViewId="0">
+    <sheetView zoomScale="41" workbookViewId="0">
       <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
@@ -6708,8 +6708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4063B8-5AB2-48E8-AFD3-3A298C84A064}">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+    <sheetView tabSelected="1" topLeftCell="M11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8739,7 +8739,7 @@
       </c>
       <c r="S27" s="1"/>
       <c r="T27" s="1" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="U27" s="1" t="s">
         <v>30</v>
@@ -8813,7 +8813,7 @@
       </c>
       <c r="S28" s="1"/>
       <c r="T28" s="1" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="U28" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Fixed an error in the week example. Also enabled error messages for weeks
</commit_message>
<xml_diff>
--- a/CampScheduler/CampScheduler/CampSchedulerInputExamples.xlsx
+++ b/CampScheduler/CampScheduler/CampSchedulerInputExamples.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dryan\OneDrive\Documents\GitHub\CampScheduler\CampScheduler\CampScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12193CC4-5B14-4972-8D4B-BDB2D637D012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BA9C34-0974-40F7-82A9-E4A3AF24C4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="1" activeTab="4" xr2:uid="{0861955A-A212-4BF4-8127-4D8CB03931E6}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="115">
   <si>
     <t>BLOCKS TABLE</t>
   </si>
@@ -379,9 +379,6 @@
   </si>
   <si>
     <t>Wednesday</t>
-  </si>
-  <si>
-    <t>1,2</t>
   </si>
   <si>
     <t>Thursday</t>
@@ -6708,8 +6705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4063B8-5AB2-48E8-AFD3-3A298C84A064}">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T29" sqref="T29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8044,7 +8041,7 @@
         <v>2</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1" t="s">
@@ -8118,7 +8115,7 @@
         <v>2</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>113</v>
+        <v>28</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1" t="s">
@@ -8464,7 +8461,7 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>27</v>
@@ -8538,7 +8535,7 @@
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>35</v>
@@ -8612,7 +8609,7 @@
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A26" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>34</v>
@@ -8686,7 +8683,7 @@
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>46</v>
@@ -8760,7 +8757,7 @@
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A28" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>39</v>
@@ -8834,7 +8831,7 @@
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>51</v>
@@ -8898,7 +8895,7 @@
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>54</v>
@@ -8962,7 +8959,7 @@
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A31" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>27</v>
@@ -9010,7 +9007,7 @@
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A32" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>35</v>
@@ -9058,7 +9055,7 @@
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A33" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>34</v>
@@ -9106,7 +9103,7 @@
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>46</v>
@@ -9154,7 +9151,7 @@
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>39</v>
@@ -9202,7 +9199,7 @@
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A36" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>51</v>
@@ -9250,7 +9247,7 @@
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A37" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Bump is now being output after generation. Fixed it around so now, counselors don't get the same activity twice (with the exception of overflows), changing room is accounted for, and did some general bug fixes so that it worked as intended. Also, update the unformat button so it now will unformat a bump output. Next time (which should be in a few hours), format bump, and do tally sheet thing. Also note for future reference, I'm going to push lunch functionality in the bump for later as its not going to be required for this upcoming summer
</commit_message>
<xml_diff>
--- a/CampScheduler/CampScheduler/CampSchedulerInputExamples.xlsx
+++ b/CampScheduler/CampScheduler/CampSchedulerInputExamples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dryan\OneDrive\Documents\GitHub\CampScheduler\CampScheduler\CampScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A831AA3-708C-4308-BF86-341250D847DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBD44EA-786E-4FB3-B084-B55F94D1640B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="3" activeTab="6" xr2:uid="{0861955A-A212-4BF4-8127-4D8CB03931E6}"/>
+    <workbookView xWindow="2588" yWindow="2498" windowWidth="16200" windowHeight="9307" firstSheet="4" activeTab="6" xr2:uid="{0861955A-A212-4BF4-8127-4D8CB03931E6}"/>
   </bookViews>
   <sheets>
     <sheet name="DayInputEmpty" sheetId="2" r:id="rId1"/>
@@ -6878,8 +6878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4063B8-5AB2-48E8-AFD3-3A298C84A064}">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9715,7 +9715,7 @@
   <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9820,7 +9820,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -9832,10 +9832,10 @@
         <v>30</v>
       </c>
       <c r="G3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>28</v>
@@ -9882,10 +9882,10 @@
         <v>30</v>
       </c>
       <c r="G4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>28</v>
@@ -10020,7 +10020,7 @@
         <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -10082,7 +10082,7 @@
         <v>30</v>
       </c>
       <c r="G8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8" s="1">
         <v>1</v>
@@ -10463,7 +10463,7 @@
         <v>2</v>
       </c>
       <c r="H17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>28</v>
@@ -10627,7 +10627,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>28</v>
@@ -10832,7 +10832,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>28</v>
@@ -10870,7 +10870,7 @@
         <v>30</v>
       </c>
       <c r="G27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H27" s="1">
         <v>1</v>
@@ -10911,7 +10911,7 @@
         <v>30</v>
       </c>
       <c r="G28" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28" s="1">
         <v>1</v>

</xml_diff>